<commit_message>
Replace entire table content to allow use of cells in template
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">The first task description</t>
   </si>
   <si>
-    <t xml:space="preserve">The second task description</t>
+    <t xml:space="preserve">The second task description is way too long to be fully shown on the description part of the sticky, but it does not push the sprint id off the sticky because that’s in a separate table cell</t>
   </si>
   <si>
     <t xml:space="preserve">some other story</t>
@@ -149,8 +149,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>